<commit_message>
Updated the writeup with the taxonomy and vectors section
</commit_message>
<xml_diff>
--- a/Source statistics.xlsx
+++ b/Source statistics.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16260" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16300" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1460,8 +1460,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G171"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="G39" sqref="G39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1911,6 +1911,10 @@
       <c r="B38" s="1">
         <v>41</v>
       </c>
+      <c r="G38">
+        <f>1126/(1126+3963)</f>
+        <v>0.22126154450776184</v>
+      </c>
     </row>
     <row r="39" spans="1:7">
       <c r="A39" t="s">

</xml_diff>